<commit_message>
- Ajout de quelques parties dans le Rapport - Modifications du changement de niveau (test d'optimisation) - Modification de la taille du titre
</commit_message>
<xml_diff>
--- a/Administration/RepartRapport.xlsx
+++ b/Administration/RepartRapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\Programmation\Projet P2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\Programmation\Projet P2\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +166,14 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,9 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +510,7 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -631,7 +640,7 @@
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MAJ: Rapport, RepartRapport, images de loutres, m_pause (Retourner au dernier Checkpoint au lieu de Redemarer le Niveau et Redemarer la partie au lieur de Redémarrer le Jeu), DELETE: Installeur des codes sources, TEST FIX: Gameboard (removeAllItems())
</commit_message>
<xml_diff>
--- a/Administration/RepartRapport.xlsx
+++ b/Administration/RepartRapport.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\Programmation\Projet P2\Administration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="9700"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -153,7 +151,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +176,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,15 +208,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -260,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,17 +501,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -503,95 +522,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="3"/>
       <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7">
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7">
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7">
       <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7">
       <c r="C12" t="s">
         <v>37</v>
       </c>
@@ -602,18 +622,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="15">
       <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="E14" t="s">
         <v>35</v>
       </c>
@@ -621,7 +641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7">
       <c r="E15" t="s">
         <v>38</v>
       </c>
@@ -629,28 +649,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7">
       <c r="G16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7">
       <c r="G17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7">
       <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:7">
       <c r="G23" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJ: README, RepartRapport, Commandes Windows, Config de l'installer windows, Gameboard header, organisation des folders AJOUTS: Licenses, Installateur windows, dlls filtrés
</commit_message>
<xml_diff>
--- a/Administration/RepartRapport.xlsx
+++ b/Administration/RepartRapport.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="B3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -615,7 +615,7 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G12" t="s">
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G14" t="s">
@@ -642,7 +642,7 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G15" t="s">

</xml_diff>

<commit_message>
- Tentative d'optimisation (DisconnectTimer) - Fonctions renommées pour mieux correspondre à leur contenu final - Ajout du nombre maximal de vies à 99 - Modification du Widget d'affichage des vies pour afficher le nombre de vies plutôt que N images
</commit_message>
<xml_diff>
--- a/Administration/RepartRapport.xlsx
+++ b/Administration/RepartRapport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Steve</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>SinkMovable</t>
-  </si>
-  <si>
-    <t>checkGameOver</t>
   </si>
   <si>
     <t>checkItem</t>
@@ -153,19 +150,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
     <font>
       <strike/>
@@ -196,10 +187,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,16 +470,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G23"/>
+  <dimension ref="B3:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -508,9 +499,9 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -519,10 +510,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -530,123 +518,123 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" t="s">
-        <v>36</v>
+      <c r="G17" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>18</v>
+      <c r="G18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>